<commit_message>
usb footprint changes, Silkscreen markers for pin 1 in ICs and polarity for other components. Edited excel BOM list and kicad list for BOM cost.
</commit_message>
<xml_diff>
--- a/stm32f429z/BOM.xlsx
+++ b/stm32f429z/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\GitHub\PCB_practice\stm32f429z\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{745C35B5-AD6E-4C25-9E40-0BEA0052F462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A78012-3AB0-41FB-8066-12C7B0D9C822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{85084DCD-3AAD-4F8C-8E9B-481F53484162}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19150" windowHeight="21000" xr2:uid="{85084DCD-3AAD-4F8C-8E9B-481F53484162}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="87">
   <si>
     <t>c1</t>
   </si>
@@ -258,13 +258,52 @@
   </si>
   <si>
     <t>C12668</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/comchip-technology/CDBA140SL-HF/3308122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External parts </t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/molex/0768250006/5639613</t>
+  </si>
+  <si>
+    <t>Molex F</t>
+  </si>
+  <si>
+    <t>Molex M</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/molex/1716920106/4515273</t>
+  </si>
+  <si>
+    <t>USB-UART</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/65100516121/4465561</t>
+  </si>
+  <si>
+    <t>USB Data</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/molex/0676432911/2421596?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-2421596_sig-Cj0KCQiAnrOtBhDIARIsAFsSe50e-lGQ2SQd1pkdFcN1TPIkQJ9f-tfYof14fjwIXYG6536pi7bZReEaAiLVEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQiAnrOtBhDIARIsAFsSe50e-lGQ2SQd1pkdFcN1TPIkQJ9f-tfYof14fjwIXYG6536pi7bZReEaAiLVEALw_wcB</t>
+  </si>
+  <si>
+    <t>USB power</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/gct/USB4085-GF-A/9859662</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +326,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -335,15 +382,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -352,10 +399,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -668,563 +715,603 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB17F14-C811-4E85-99FC-2E9C88686FD9}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="44.08984375" customWidth="1"/>
+    <col min="4" max="4" width="78.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="5"/>
       <c r="C1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="3"/>
       <c r="C5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="3"/>
       <c r="C6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="3"/>
       <c r="C7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="3"/>
       <c r="C8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="3"/>
       <c r="C9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="3"/>
       <c r="C10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="3"/>
       <c r="C11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="3"/>
       <c r="C12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="3"/>
       <c r="C13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="3"/>
       <c r="C14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="3"/>
       <c r="C15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="5" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="3"/>
       <c r="C17" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="6" t="s">
+      <c r="B18" s="3"/>
+      <c r="C18" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="3"/>
+      <c r="C19" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="3"/>
+      <c r="C20" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="3"/>
       <c r="C21" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="3"/>
       <c r="C22" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="2"/>
+      <c r="B23" s="3"/>
       <c r="C23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="3"/>
       <c r="C24" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="6" t="s">
+      <c r="B25" s="3"/>
+      <c r="C25" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="3"/>
       <c r="C26" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="6" t="s">
+      <c r="B27" s="3"/>
+      <c r="C27" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="6" t="s">
+      <c r="B28" s="3"/>
+      <c r="C28" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="2"/>
+      <c r="B29" s="3"/>
       <c r="C29" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="3"/>
       <c r="C30" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="3"/>
       <c r="C31" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="5" t="s">
+      <c r="B32" s="3"/>
+      <c r="C32" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="1"/>
+      <c r="B33" s="3"/>
       <c r="C33" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="1"/>
+      <c r="B34" s="3"/>
       <c r="C34" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="1"/>
+      <c r="B35" s="3"/>
       <c r="C35" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A36" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="5" t="s">
+      <c r="B36" s="3"/>
+      <c r="C36" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="1" t="s">
+      <c r="D36" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A37" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="5" t="s">
+      <c r="B37" s="3"/>
+      <c r="C37" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
+      <c r="D37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="6" t="s">
+      <c r="B39" s="3"/>
+      <c r="C39" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="1"/>
+      <c r="B40" s="3"/>
       <c r="C40" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="1"/>
+      <c r="B41" s="3"/>
       <c r="C41" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B42" s="1"/>
+      <c r="B42" s="3"/>
       <c r="C42" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="6" t="s">
+      <c r="B43" s="3"/>
+      <c r="C43" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B44" s="1"/>
+      <c r="B44" s="3"/>
       <c r="C44" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B45" s="1"/>
+      <c r="B45" s="3"/>
       <c r="C45" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B46" s="1"/>
+      <c r="B46" s="3"/>
       <c r="C46" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B47" s="1"/>
-      <c r="C47" s="6" t="s">
+      <c r="B47" s="3"/>
+      <c r="C47" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B48" s="1"/>
-      <c r="C48" s="6" t="s">
+      <c r="B48" s="3"/>
+      <c r="C48" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="6" t="s">
+      <c r="B49" s="3"/>
+      <c r="C49" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B50" s="1"/>
-      <c r="C50" s="6" t="s">
+      <c r="B50" s="3"/>
+      <c r="C50" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B51" s="1"/>
+      <c r="B51" s="3"/>
       <c r="C51" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B52" s="1"/>
+      <c r="B52" s="3"/>
       <c r="C52" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B53" s="1"/>
+      <c r="B53" s="3"/>
       <c r="C53" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B54" s="1"/>
+      <c r="B54" s="3"/>
       <c r="C54" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="6" t="s">
+      <c r="B55" s="3"/>
+      <c r="C55" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B56" s="1"/>
+      <c r="B56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B57" s="3"/>
+      <c r="D57" t="s">
+        <v>77</v>
+      </c>
+      <c r="E57">
+        <f>3.17 *6</f>
+        <v>19.02</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="D58" t="s">
+        <v>80</v>
+      </c>
+      <c r="E58">
+        <f>1.28 * 6</f>
+        <v>7.68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B59" s="3"/>
+      <c r="D59" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E59">
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="D60" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E60">
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="D61" t="s">
+        <v>86</v>
+      </c>
+      <c r="E61">
+        <v>0.94</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
+  <mergeCells count="61">
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
@@ -1235,8 +1322,58 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D60" r:id="rId1" display="https://www.digikey.com/en/products/detail/molex/0676432911/2421596?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-2421596_sig-Cj0KCQiAnrOtBhDIARIsAFsSe50e-lGQ2SQd1pkdFcN1TPIkQJ9f-tfYof14fjwIXYG6536pi7bZReEaAiLVEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQiAnrOtBhDIARIsAFsSe50e-lGQ2SQd1pkdFcN1TPIkQJ9f-tfYof14fjwIXYG6536pi7bZReEaAiLVEALw_wcB" xr:uid="{96BE2175-809E-460E-B79E-E718E4734926}"/>
+    <hyperlink ref="D59" r:id="rId2" xr:uid="{E460B263-F1DF-4915-94D2-37F9F3C4E350}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
redid the manufacturing folder to get it to be compatible with JLC
</commit_message>
<xml_diff>
--- a/stm32f429z/BOM.xlsx
+++ b/stm32f429z/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\GitHub\PCB_practice\stm32f429z\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A78012-3AB0-41FB-8066-12C7B0D9C822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB659A2-EB63-4330-A507-8B8D4966B551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19150" windowHeight="21000" xr2:uid="{85084DCD-3AAD-4F8C-8E9B-481F53484162}"/>
+    <workbookView xWindow="13860" yWindow="4090" windowWidth="21520" windowHeight="15100" xr2:uid="{85084DCD-3AAD-4F8C-8E9B-481F53484162}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -390,6 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -399,7 +400,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -715,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB17F14-C811-4E85-99FC-2E9C88686FD9}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -728,10 +728,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="6"/>
       <c r="C1" t="s">
         <v>31</v>
       </c>
@@ -743,316 +743,316 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="4"/>
       <c r="C5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="4"/>
       <c r="C6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="4"/>
       <c r="C7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="4"/>
       <c r="C8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="4"/>
       <c r="C9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="4"/>
       <c r="C10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="4"/>
       <c r="C11" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="4"/>
       <c r="C12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="4"/>
       <c r="C13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="4"/>
       <c r="C14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="4"/>
       <c r="C15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B17" s="4"/>
       <c r="C17" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="4"/>
       <c r="C18" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="3"/>
+      <c r="B19" s="4"/>
       <c r="C19" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="3"/>
+      <c r="B20" s="4"/>
       <c r="C20" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="3"/>
+      <c r="B21" s="4"/>
       <c r="C21" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="3"/>
+      <c r="B22" s="4"/>
       <c r="C22" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="3"/>
+      <c r="B23" s="4"/>
       <c r="C23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="4"/>
       <c r="C24" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="3"/>
+      <c r="B25" s="4"/>
       <c r="C25" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="3"/>
+      <c r="B26" s="4"/>
       <c r="C26" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="3"/>
+      <c r="B27" s="4"/>
       <c r="C27" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="3"/>
+      <c r="B28" s="4"/>
       <c r="C28" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="3"/>
+      <c r="B29" s="4"/>
       <c r="C29" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="3"/>
+      <c r="B30" s="4"/>
       <c r="C30" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="3"/>
+      <c r="B31" s="4"/>
       <c r="C31" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="3"/>
+      <c r="B32" s="4"/>
       <c r="C32" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="3"/>
+      <c r="B33" s="4"/>
       <c r="C33" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="3"/>
+      <c r="B34" s="4"/>
       <c r="C34" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="3"/>
+      <c r="B35" s="4"/>
       <c r="C35" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="3"/>
+      <c r="B36" s="4"/>
       <c r="C36" s="1" t="s">
         <v>48</v>
       </c>
@@ -1064,10 +1064,10 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="3"/>
+      <c r="B37" s="4"/>
       <c r="C37" s="1" t="s">
         <v>48</v>
       </c>
@@ -1079,175 +1079,175 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="3"/>
+      <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="3"/>
+      <c r="B39" s="4"/>
       <c r="C39" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="3"/>
+      <c r="B40" s="4"/>
       <c r="C40" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="3"/>
+      <c r="B41" s="4"/>
       <c r="C41" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B42" s="3"/>
+      <c r="B42" s="4"/>
       <c r="C42" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B43" s="3"/>
+      <c r="B43" s="4"/>
       <c r="C43" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B44" s="3"/>
+      <c r="B44" s="4"/>
       <c r="C44" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B45" s="3"/>
+      <c r="B45" s="4"/>
       <c r="C45" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B46" s="3"/>
+      <c r="B46" s="4"/>
       <c r="C46" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B47" s="3"/>
+      <c r="B47" s="4"/>
       <c r="C47" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B48" s="3"/>
+      <c r="B48" s="4"/>
       <c r="C48" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B49" s="3"/>
+      <c r="B49" s="4"/>
       <c r="C49" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B50" s="3"/>
+      <c r="B50" s="4"/>
       <c r="C50" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B51" s="3"/>
+      <c r="B51" s="4"/>
       <c r="C51" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B52" s="3"/>
+      <c r="B52" s="4"/>
       <c r="C52" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B53" s="3"/>
+      <c r="B53" s="4"/>
       <c r="C53" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B54" s="3"/>
+      <c r="B54" s="4"/>
       <c r="C54" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B55" s="3"/>
+      <c r="B55" s="4"/>
       <c r="C55" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B56" s="3"/>
+      <c r="B56" s="4"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B57" s="3"/>
+      <c r="B57" s="4"/>
       <c r="D57" t="s">
         <v>77</v>
       </c>
@@ -1257,10 +1257,10 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B58" s="3"/>
+      <c r="B58" s="4"/>
       <c r="D58" t="s">
         <v>80</v>
       </c>
@@ -1270,11 +1270,11 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B59" s="3"/>
-      <c r="D59" s="6" t="s">
+      <c r="B59" s="4"/>
+      <c r="D59" s="3" t="s">
         <v>82</v>
       </c>
       <c r="E59">
@@ -1282,11 +1282,11 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B60" s="3"/>
-      <c r="D60" s="6" t="s">
+      <c r="B60" s="4"/>
+      <c r="D60" s="3" t="s">
         <v>84</v>
       </c>
       <c r="E60">
@@ -1294,10 +1294,10 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="3"/>
+      <c r="B61" s="4"/>
       <c r="D61" t="s">
         <v>86</v>
       </c>
@@ -1305,13 +1305,55 @@
         <v>0.94</v>
       </c>
     </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E62">
+        <f>E57+E58+E60+E59+E61+E36+E37</f>
+        <v>32.39</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
@@ -1327,47 +1369,11 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>